<commit_message>
Updated test plan after fixing bugs
</commit_message>
<xml_diff>
--- a/documentation/CS411 Test Plan.xlsx
+++ b/documentation/CS411 Test Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3260" yWindow="0" windowWidth="24620" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Field Validations" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="104">
   <si>
     <t>Page name</t>
   </si>
@@ -54,266 +54,298 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>sopiegpoegkp</t>
-  </si>
-  <si>
     <t>**</t>
   </si>
   <si>
-    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
     <t>radiohead</t>
   </si>
   <si>
     <t>å</t>
   </si>
   <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>"        "</t>
   </si>
   <si>
-    <t>login.textinput1</t>
-  </si>
-  <si>
-    <t>login.textinput2</t>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Read/Write</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>String &lt; 200</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>UI Element</t>
+  </si>
+  <si>
+    <t>Expected Function</t>
+  </si>
+  <si>
+    <t>BugID</t>
+  </si>
+  <si>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Severity (1 to 3)</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>authenticate with twitter</t>
+  </si>
+  <si>
+    <t>ui1</t>
+  </si>
+  <si>
+    <t>ui2</t>
+  </si>
+  <si>
+    <t>ui3</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>field3</t>
+  </si>
+  <si>
+    <t>field4</t>
+  </si>
+  <si>
+    <t>field5</t>
+  </si>
+  <si>
+    <t>field6</t>
+  </si>
+  <si>
+    <t>field7</t>
+  </si>
+  <si>
+    <t>field8</t>
+  </si>
+  <si>
+    <t>field9</t>
+  </si>
+  <si>
+    <t>field10</t>
+  </si>
+  <si>
+    <t>field11</t>
+  </si>
+  <si>
+    <t>Tweet</t>
+  </si>
+  <si>
+    <t>Search for User</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Read/Write</t>
-  </si>
-  <si>
-    <t>Twitter Password</t>
-  </si>
-  <si>
-    <t>Data Source</t>
-  </si>
-  <si>
-    <t>Constraints</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>social_id</t>
-  </si>
-  <si>
-    <t>is_authenticated</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>String &lt; 200</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>True or False</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>data2</t>
-  </si>
-  <si>
-    <t>data3</t>
-  </si>
-  <si>
-    <t>Page Name</t>
-  </si>
-  <si>
-    <t>UI Element</t>
-  </si>
-  <si>
-    <t>Expected Function</t>
-  </si>
-  <si>
-    <t>BugID</t>
-  </si>
-  <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Severity (1 to 3)</t>
-  </si>
-  <si>
-    <t>Assigned</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>authenticate with twitter</t>
-  </si>
-  <si>
-    <t>Create Post</t>
-  </si>
-  <si>
-    <t>Genarate Paragraph</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
-    <t>ui1</t>
-  </si>
-  <si>
-    <t>ui2</t>
-  </si>
-  <si>
-    <t>ui3</t>
-  </si>
-  <si>
-    <t>field1</t>
-  </si>
-  <si>
-    <t>field2</t>
-  </si>
-  <si>
-    <t>field3</t>
-  </si>
-  <si>
-    <t>field4</t>
-  </si>
-  <si>
-    <t>field5</t>
-  </si>
-  <si>
-    <t>field6</t>
-  </si>
-  <si>
-    <t>field7</t>
-  </si>
-  <si>
-    <t>field8</t>
-  </si>
-  <si>
-    <t>field9</t>
-  </si>
-  <si>
-    <t>field10</t>
-  </si>
-  <si>
-    <t>field11</t>
-  </si>
-  <si>
-    <t>wordcloud</t>
-  </si>
-  <si>
-    <t>faketweets</t>
-  </si>
-  <si>
-    <t>w/r</t>
-  </si>
-  <si>
-    <t>twitter.json</t>
-  </si>
-  <si>
-    <t>String &lt; 10000</t>
-  </si>
-  <si>
-    <t>String &lt; 260</t>
-  </si>
-  <si>
-    <t>data4</t>
-  </si>
-  <si>
-    <t>data5</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>select option to create fake post</t>
-  </si>
-  <si>
-    <t>select option to create fake paragraph</t>
-  </si>
-  <si>
-    <t>create option above</t>
-  </si>
-  <si>
-    <t>ui4</t>
-  </si>
-  <si>
-    <t>login.boolean1</t>
-  </si>
-  <si>
-    <t>goagain</t>
-  </si>
-  <si>
-    <t>Create another post</t>
-  </si>
-  <si>
-    <t>sends user back to home page</t>
-  </si>
-  <si>
-    <t>ui5</t>
-  </si>
-  <si>
-    <t>bug1</t>
-  </si>
-  <si>
-    <t>bug2</t>
-  </si>
-  <si>
-    <t>bug3</t>
-  </si>
-  <si>
-    <t>should return "invalid user" when passed whitespace characters</t>
-  </si>
-  <si>
-    <t>should return "invalid user" when passed whitespace characters surrounded by quotes</t>
-  </si>
-  <si>
-    <t>"    zzzzz    "</t>
-  </si>
-  <si>
-    <t>should return "invalid user" when passed whitespace characters followed by a string, surrounded by quotes</t>
+    <t>Sign Out</t>
+  </si>
+  <si>
+    <t>Tweets</t>
+  </si>
+  <si>
+    <t>r/w</t>
+  </si>
+  <si>
+    <t>tweet</t>
+  </si>
+  <si>
+    <t>home.user</t>
+  </si>
+  <si>
+    <t>home.tweet</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>String &lt; 240</t>
+  </si>
+  <si>
+    <t>segegegoegjoejoegj</t>
+  </si>
+  <si>
+    <t>Sign in with Twitter</t>
+  </si>
+  <si>
+    <t>home.tweethere</t>
+  </si>
+  <si>
+    <t>home.searchuser</t>
+  </si>
+  <si>
+    <t>field12</t>
+  </si>
+  <si>
+    <t>field13</t>
+  </si>
+  <si>
+    <t>field14</t>
+  </si>
+  <si>
+    <t>field15</t>
+  </si>
+  <si>
+    <t>field16</t>
+  </si>
+  <si>
+    <t>field17</t>
+  </si>
+  <si>
+    <t>field18</t>
+  </si>
+  <si>
+    <t>field19</t>
+  </si>
+  <si>
+    <t>field20</t>
+  </si>
+  <si>
+    <t>field21</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        /</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user"</t>
+  </si>
+  <si>
+    <t>posts new tweet</t>
+  </si>
+  <si>
+    <t>logs you out of twitter</t>
+  </si>
+  <si>
+    <t>searches for user</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed invalid user (segegegoegjoejoegj)</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed int</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed special characters (**)</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed empty quotes</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed .</t>
+  </si>
+  <si>
+    <t>you're so vain, you probably think this tweet is about you</t>
+  </si>
+  <si>
+    <t>#noonewillnotice #noonewillknow</t>
+  </si>
+  <si>
+    <t>""sweet dark</t>
+  </si>
+  <si>
+    <t>over 240 characters, doesn’t post</t>
+  </si>
+  <si>
+    <t>!@#$%^</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>when the cool of the pond makes you drop down on it, when the smell of the lawn makes you flop down on it, when the teenage car gets the cop down on it, that time is here for one more year, and that summer feeling is gonna haunt you for the rest of your life and then that summer feelings gonna taunt ya! and then that summer feeling is gonna hurt you one day in your life</t>
+  </si>
+  <si>
+    <t>Should indicate "invalid user" when passed special characters (å)</t>
+  </si>
+  <si>
+    <t>^&amp;*#$%^</t>
+  </si>
+  <si>
+    <t>bug1.1</t>
+  </si>
+  <si>
+    <t>bug1.2</t>
+  </si>
+  <si>
+    <t>bug1.3</t>
+  </si>
+  <si>
+    <t>bug1.4</t>
+  </si>
+  <si>
+    <t>bug1.5</t>
+  </si>
+  <si>
+    <t>bug1.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -342,6 +374,13 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -360,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,16 +419,76 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -399,6 +498,34 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -408,6 +535,34 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -737,21 +892,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,19 +927,22 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -791,198 +951,425 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="135">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18">
+        <v>123456789</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>91</v>
       </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -998,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1013,22 +1400,22 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1039,117 +1426,54 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1165,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1179,13 +1503,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1196,16 +1520,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1213,13 +1540,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1227,13 +1557,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1241,27 +1574,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" t="s">
-        <v>85</v>
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1276,78 +1598,156 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="71.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="5">
+        <v>43080</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>